<commit_message>
Table for summary of lengths has been moved further up in the script and has been adapted, so lengths are now FL for both stereo-DOVs and UVC.
</commit_message>
<xml_diff>
--- a/Tables/Summary_lengths.xlsx
+++ b/Tables/Summary_lengths.xlsx
@@ -26,13 +26,13 @@
     <t xml:space="preserve">minFL_DOVS</t>
   </si>
   <si>
-    <t xml:space="preserve">minTL_UVC</t>
+    <t xml:space="preserve">minFL_UVC</t>
   </si>
   <si>
     <t xml:space="preserve">maxFL_DOVS</t>
   </si>
   <si>
-    <t xml:space="preserve">maxTL_UVC</t>
+    <t xml:space="preserve">maxFL_UVC</t>
   </si>
   <si>
     <t xml:space="preserve">meanFL_DOVS</t>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">SE_DOVS</t>
   </si>
   <si>
-    <t xml:space="preserve">meanTL_UVC</t>
+    <t xml:space="preserve">meanFL_UVC</t>
   </si>
   <si>
     <t xml:space="preserve">SE_UVC</t>
@@ -543,27 +543,19 @@
       <c r="D3" t="n">
         <v>244</v>
       </c>
-      <c r="E3" t="n">
-        <v>400</v>
-      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
         <v>465</v>
       </c>
-      <c r="G3" t="n">
-        <v>500</v>
-      </c>
+      <c r="G3"/>
       <c r="H3" t="n">
         <v>404</v>
       </c>
       <c r="I3" t="n">
         <v>22.68</v>
       </c>
-      <c r="J3" t="n">
-        <v>433</v>
-      </c>
-      <c r="K3" t="n">
-        <v>33.33</v>
-      </c>
+      <c r="J3"/>
+      <c r="K3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -574,21 +566,13 @@
         <v>50</v>
       </c>
       <c r="D4"/>
-      <c r="E4" t="n">
-        <v>400</v>
-      </c>
+      <c r="E4"/>
       <c r="F4"/>
-      <c r="G4" t="n">
-        <v>400</v>
-      </c>
+      <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="J4" t="n">
-        <v>400</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
+      <c r="J4"/>
+      <c r="K4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -599,21 +583,13 @@
         <v>40</v>
       </c>
       <c r="D5"/>
-      <c r="E5" t="n">
-        <v>700</v>
-      </c>
+      <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" t="n">
-        <v>700</v>
-      </c>
+      <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
-      <c r="J5" t="n">
-        <v>700</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
+      <c r="J5"/>
+      <c r="K5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -629,13 +605,13 @@
         <v>434</v>
       </c>
       <c r="E6" t="n">
-        <v>400</v>
+        <v>345</v>
       </c>
       <c r="F6" t="n">
         <v>640</v>
       </c>
       <c r="G6" t="n">
-        <v>800</v>
+        <v>690</v>
       </c>
       <c r="H6" t="n">
         <v>542</v>
@@ -644,10 +620,10 @@
         <v>25.57</v>
       </c>
       <c r="J6" t="n">
-        <v>546</v>
+        <v>471</v>
       </c>
       <c r="K6" t="n">
-        <v>44.74</v>
+        <v>38.61</v>
       </c>
     </row>
     <row r="7">
@@ -664,13 +640,13 @@
         <v>648</v>
       </c>
       <c r="E7" t="n">
-        <v>500</v>
+        <v>468</v>
       </c>
       <c r="F7" t="n">
         <v>811</v>
       </c>
       <c r="G7" t="n">
-        <v>800</v>
+        <v>749</v>
       </c>
       <c r="H7" t="n">
         <v>732</v>
@@ -679,10 +655,10 @@
         <v>12.82</v>
       </c>
       <c r="J7" t="n">
-        <v>641</v>
+        <v>600</v>
       </c>
       <c r="K7" t="n">
-        <v>18.21</v>
+        <v>17.05</v>
       </c>
     </row>
     <row r="8">
@@ -694,18 +670,12 @@
         <v>1</v>
       </c>
       <c r="D8"/>
-      <c r="E8" t="n">
-        <v>2000</v>
-      </c>
+      <c r="E8"/>
       <c r="F8"/>
-      <c r="G8" t="n">
-        <v>2000</v>
-      </c>
+      <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8" t="n">
-        <v>2000</v>
-      </c>
+      <c r="J8"/>
       <c r="K8"/>
     </row>
     <row r="9">
@@ -722,13 +692,13 @@
         <v>618</v>
       </c>
       <c r="E9" t="n">
-        <v>800</v>
+        <v>647</v>
       </c>
       <c r="F9" t="n">
         <v>2624</v>
       </c>
       <c r="G9" t="n">
-        <v>3000</v>
+        <v>2425</v>
       </c>
       <c r="H9" t="n">
         <v>1562</v>
@@ -737,10 +707,10 @@
         <v>61.34</v>
       </c>
       <c r="J9" t="n">
-        <v>1811</v>
+        <v>1464</v>
       </c>
       <c r="K9" t="n">
-        <v>49.29</v>
+        <v>39.85</v>
       </c>
     </row>
     <row r="10">
@@ -757,13 +727,13 @@
         <v>1619</v>
       </c>
       <c r="E10" t="n">
-        <v>1750</v>
+        <v>1445</v>
       </c>
       <c r="F10" t="n">
         <v>2247</v>
       </c>
       <c r="G10" t="n">
-        <v>2500</v>
+        <v>2064</v>
       </c>
       <c r="H10" t="n">
         <v>1933</v>
@@ -772,10 +742,10 @@
         <v>314.37</v>
       </c>
       <c r="J10" t="n">
-        <v>2062</v>
+        <v>1703</v>
       </c>
       <c r="K10" t="n">
-        <v>157.29</v>
+        <v>129.88</v>
       </c>
     </row>
     <row r="11">
@@ -826,27 +796,19 @@
       <c r="D12" t="n">
         <v>572</v>
       </c>
-      <c r="E12" t="n">
-        <v>500</v>
-      </c>
+      <c r="E12"/>
       <c r="F12" t="n">
         <v>640</v>
       </c>
-      <c r="G12" t="n">
-        <v>600</v>
-      </c>
+      <c r="G12"/>
       <c r="H12" t="n">
         <v>628</v>
       </c>
       <c r="I12" t="n">
         <v>7.15</v>
       </c>
-      <c r="J12" t="n">
-        <v>533</v>
-      </c>
-      <c r="K12" t="n">
-        <v>33.33</v>
-      </c>
+      <c r="J12"/>
+      <c r="K12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -861,27 +823,19 @@
       <c r="D13" t="n">
         <v>388</v>
       </c>
-      <c r="E13" t="n">
-        <v>800</v>
-      </c>
+      <c r="E13"/>
       <c r="F13" t="n">
         <v>593</v>
       </c>
-      <c r="G13" t="n">
-        <v>800</v>
-      </c>
+      <c r="G13"/>
       <c r="H13" t="n">
         <v>503</v>
       </c>
       <c r="I13" t="n">
         <v>22.93</v>
       </c>
-      <c r="J13" t="n">
-        <v>800</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
+      <c r="J13"/>
+      <c r="K13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -897,13 +851,13 @@
         <v>479</v>
       </c>
       <c r="E14" t="n">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="F14" t="n">
         <v>836</v>
       </c>
       <c r="G14" t="n">
-        <v>800</v>
+        <v>768</v>
       </c>
       <c r="H14" t="n">
         <v>629</v>
@@ -912,10 +866,10 @@
         <v>64.55</v>
       </c>
       <c r="J14" t="n">
-        <v>583</v>
+        <v>560</v>
       </c>
       <c r="K14" t="n">
-        <v>23.05</v>
+        <v>22.14</v>
       </c>
     </row>
     <row r="15">
@@ -962,18 +916,12 @@
         <v>1</v>
       </c>
       <c r="D16"/>
-      <c r="E16" t="n">
-        <v>1000</v>
-      </c>
+      <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="n">
-        <v>1000</v>
-      </c>
+      <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
-      <c r="J16" t="n">
-        <v>1000</v>
-      </c>
+      <c r="J16"/>
       <c r="K16"/>
     </row>
     <row r="17">
@@ -990,13 +938,13 @@
         <v>134</v>
       </c>
       <c r="E17" t="n">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="F17" t="n">
         <v>698</v>
       </c>
       <c r="G17" t="n">
-        <v>700</v>
+        <v>671</v>
       </c>
       <c r="H17" t="n">
         <v>384</v>
@@ -1005,10 +953,10 @@
         <v>3.41</v>
       </c>
       <c r="J17" t="n">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="K17" t="n">
-        <v>4.35</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="18">
@@ -1025,13 +973,13 @@
         <v>329</v>
       </c>
       <c r="E18" t="n">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="F18" t="n">
         <v>1490</v>
       </c>
       <c r="G18" t="n">
-        <v>1100</v>
+        <v>1055</v>
       </c>
       <c r="H18" t="n">
         <v>621</v>
@@ -1040,10 +988,10 @@
         <v>24.16</v>
       </c>
       <c r="J18" t="n">
-        <v>614</v>
+        <v>589</v>
       </c>
       <c r="K18" t="n">
-        <v>19.04</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="19">
@@ -1059,22 +1007,16 @@
       <c r="D19" t="n">
         <v>867</v>
       </c>
-      <c r="E19" t="n">
-        <v>3500</v>
-      </c>
+      <c r="E19"/>
       <c r="F19" t="n">
         <v>867</v>
       </c>
-      <c r="G19" t="n">
-        <v>3500</v>
-      </c>
+      <c r="G19"/>
       <c r="H19" t="n">
         <v>867</v>
       </c>
       <c r="I19"/>
-      <c r="J19" t="n">
-        <v>3500</v>
-      </c>
+      <c r="J19"/>
       <c r="K19"/>
     </row>
     <row r="20">
@@ -1091,13 +1033,13 @@
         <v>226</v>
       </c>
       <c r="E20" t="n">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="F20" t="n">
         <v>1060</v>
       </c>
       <c r="G20" t="n">
-        <v>900</v>
+        <v>878</v>
       </c>
       <c r="H20" t="n">
         <v>472</v>
@@ -1106,10 +1048,10 @@
         <v>5.22</v>
       </c>
       <c r="J20" t="n">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="K20" t="n">
-        <v>6.11</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="21">
@@ -1156,21 +1098,13 @@
         <v>3</v>
       </c>
       <c r="D22"/>
-      <c r="E22" t="n">
-        <v>700</v>
-      </c>
+      <c r="E22"/>
       <c r="F22"/>
-      <c r="G22" t="n">
-        <v>700</v>
-      </c>
+      <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
-      <c r="J22" t="n">
-        <v>700</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
+      <c r="J22"/>
+      <c r="K22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -1181,21 +1115,13 @@
         <v>9</v>
       </c>
       <c r="D23"/>
-      <c r="E23" t="n">
-        <v>800</v>
-      </c>
+      <c r="E23"/>
       <c r="F23"/>
-      <c r="G23" t="n">
-        <v>900</v>
-      </c>
+      <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23" t="n">
-        <v>889</v>
-      </c>
-      <c r="K23" t="n">
-        <v>11.11</v>
-      </c>
+      <c r="J23"/>
+      <c r="K23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -1211,13 +1137,13 @@
         <v>144</v>
       </c>
       <c r="E24" t="n">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="F24" t="n">
         <v>822</v>
       </c>
       <c r="G24" t="n">
-        <v>1000</v>
+        <v>903</v>
       </c>
       <c r="H24" t="n">
         <v>282</v>
@@ -1226,10 +1152,10 @@
         <v>43.96</v>
       </c>
       <c r="J24" t="n">
-        <v>640</v>
+        <v>578</v>
       </c>
       <c r="K24" t="n">
-        <v>51.46</v>
+        <v>46.48</v>
       </c>
     </row>
     <row r="25">
@@ -1246,13 +1172,13 @@
         <v>976</v>
       </c>
       <c r="E25" t="n">
-        <v>1250</v>
+        <v>969</v>
       </c>
       <c r="F25" t="n">
         <v>3640</v>
       </c>
       <c r="G25" t="n">
-        <v>2500</v>
+        <v>1939</v>
       </c>
       <c r="H25" t="n">
         <v>2001</v>
@@ -1261,10 +1187,10 @@
         <v>25.7</v>
       </c>
       <c r="J25" t="n">
-        <v>2047</v>
+        <v>1587</v>
       </c>
       <c r="K25" t="n">
-        <v>15.93</v>
+        <v>12.36</v>
       </c>
     </row>
     <row r="26">
@@ -1280,27 +1206,19 @@
       <c r="D26" t="n">
         <v>717</v>
       </c>
-      <c r="E26" t="n">
-        <v>700</v>
-      </c>
+      <c r="E26"/>
       <c r="F26" t="n">
         <v>1277</v>
       </c>
-      <c r="G26" t="n">
-        <v>900</v>
-      </c>
+      <c r="G26"/>
       <c r="H26" t="n">
         <v>965</v>
       </c>
       <c r="I26" t="n">
         <v>116.15</v>
       </c>
-      <c r="J26" t="n">
-        <v>838</v>
-      </c>
-      <c r="K26" t="n">
-        <v>26.31</v>
-      </c>
+      <c r="J26"/>
+      <c r="K26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -1311,18 +1229,12 @@
         <v>1</v>
       </c>
       <c r="D27"/>
-      <c r="E27" t="n">
-        <v>700</v>
-      </c>
+      <c r="E27"/>
       <c r="F27"/>
-      <c r="G27" t="n">
-        <v>700</v>
-      </c>
+      <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27" t="n">
-        <v>700</v>
-      </c>
+      <c r="J27"/>
       <c r="K27"/>
     </row>
     <row r="28">
@@ -1334,21 +1246,13 @@
         <v>2</v>
       </c>
       <c r="D28"/>
-      <c r="E28" t="n">
-        <v>800</v>
-      </c>
+      <c r="E28"/>
       <c r="F28"/>
-      <c r="G28" t="n">
-        <v>1250</v>
-      </c>
+      <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28" t="n">
-        <v>1025</v>
-      </c>
-      <c r="K28" t="n">
-        <v>225</v>
-      </c>
+      <c r="J28"/>
+      <c r="K28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -1364,13 +1268,13 @@
         <v>1042</v>
       </c>
       <c r="E29" t="n">
-        <v>1100</v>
+        <v>905</v>
       </c>
       <c r="F29" t="n">
         <v>1938</v>
       </c>
       <c r="G29" t="n">
-        <v>1750</v>
+        <v>1439</v>
       </c>
       <c r="H29" t="n">
         <v>1340</v>
@@ -1379,10 +1283,10 @@
         <v>93.25</v>
       </c>
       <c r="J29" t="n">
-        <v>1428</v>
+        <v>1174</v>
       </c>
       <c r="K29" t="n">
-        <v>40.3</v>
+        <v>33.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>